<commit_message>
favorites fixed, catalog moved to enhancer
</commit_message>
<xml_diff>
--- a/Temp/To-Fix.xlsx
+++ b/Temp/To-Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VLAD\IT\DAN_IT\FEM3-FINAL-PROJECT\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE861AC-1EB8-4AF9-8C9E-9EEDEB156A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B4BEAF-E598-48F6-959F-E961695EC132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F003A8AA-A7D0-4069-AA6E-59105AA6D065}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Filter" sheetId="1" r:id="rId1"/>
     <sheet name="General" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">General!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>собирать реальные данные с фильтра</t>
   </si>
@@ -88,13 +91,169 @@
   </si>
   <si>
     <t>Home page</t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Стиль кнопки Favourites</t>
+  </si>
+  <si>
+    <t>Wishlist</t>
+  </si>
+  <si>
+    <t>Последний элемент из wishlist не удаляется</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Where</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>deploy on HEROKU</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>code refactor</t>
+  </si>
+  <si>
+    <t>Сообщение что  в корзине ничего нет</t>
+  </si>
+  <si>
+    <t>Login/Logout</t>
+  </si>
+  <si>
+    <t>При логине и логауте текуий роут надо перезагружать (например, чтоб обновлялась корзина)</t>
+  </si>
+  <si>
+    <t>Добавить контейнер</t>
+  </si>
+  <si>
+    <t>показывать кол-ва на Favorites icon</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Обрабатывать клик "добавление в избранное" для незалогиненого пользователя - модалка</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>долго загружаются иконки категорий</t>
+  </si>
+  <si>
+    <t>Catalog</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Выбор цены не работает</t>
+  </si>
+  <si>
+    <t>Выбор цены сделать более симпатичным</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Адаптивность</t>
+  </si>
+  <si>
+    <t>Выезд поля инпута по нажатию, свертка по дефокусу или переходу на другую страницу</t>
+  </si>
+  <si>
+    <t>Изменение иконки и подписи при логине/логауте</t>
+  </si>
+  <si>
+    <t>Навесить функционал логаута</t>
+  </si>
+  <si>
+    <t>Тестирование функционала на мобилке</t>
+  </si>
+  <si>
+    <t>Тестирование функционала на десктопе</t>
+  </si>
+  <si>
+    <t>Тестирование функционала на планшете</t>
+  </si>
+  <si>
+    <t>Выложить на HEROKU</t>
+  </si>
+  <si>
+    <t>Тестирование адаптивности на мобилке</t>
+  </si>
+  <si>
+    <t>Тестирование адаптивности на планшете</t>
+  </si>
+  <si>
+    <t>Тестирование адаптивности на десктопе</t>
+  </si>
+  <si>
+    <t>Обработка ошибок (.error, try catch)</t>
+  </si>
+  <si>
+    <t>Убрать ошибки eslint</t>
+  </si>
+  <si>
+    <t>Рефакторинг кода (улучшить)</t>
+  </si>
+  <si>
+    <t>Перенести все страницы в одну папку</t>
+  </si>
+  <si>
+    <t>Заменить sign Up на Register</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Сверстать чекаут</t>
+  </si>
+  <si>
+    <t>Настроить валидацию чекаут</t>
+  </si>
+  <si>
+    <t>Подтянуть данные в форму</t>
+  </si>
+  <si>
+    <t>Функционал чекаута</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +262,25 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +293,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,13 +308,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,31 +765,1189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B89314-F863-48FB-9933-FEF9A79509A7}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.5546875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="7"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="7"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="7"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="7"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="7"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="7"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="7"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="7"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="7"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="7"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="7"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="7"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="7"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="7"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="7"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="7"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="7"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="7"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="7"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="7"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="7"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="7"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="7"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="7"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="7"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="7"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="7"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="7"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="7"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="7"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="7"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="7"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="7"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="7"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="7"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="7"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="7"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="7"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="7"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="7"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="4"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="7"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="7"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="4"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="7"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="4"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="7"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="7"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="7"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="7"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="4"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="7"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="4"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="7"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="7"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="4"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="7"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="4"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="7"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="4"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="7"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="7"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="4"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" s="7"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="4"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="7"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="4"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="7"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="4"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="7"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="4"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" s="7"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="4"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" s="7"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="4"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" s="7"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="7"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="4"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" s="7"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="4"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" s="7"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="4"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126" s="7"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="4"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" s="7"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="4"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128" s="7"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="4"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" s="7"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="4"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" s="7"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="4"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" s="7"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A132" s="7"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="4"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A133" s="7"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="4"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134" s="7"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="4"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" s="7"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{97C115AA-75BA-4ECA-A4DD-57A795D89F11}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed crash on product page, search, slider
</commit_message>
<xml_diff>
--- a/Temp/To-Fix.xlsx
+++ b/Temp/To-Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VLAD\IT\DAN_IT\FEM3-FINAL-PROJECT\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF84B4D-98CD-419A-9945-880ED8923324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1354E0A0-B883-4045-BF73-9B290D936DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F003A8AA-A7D0-4069-AA6E-59105AA6D065}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="210">
   <si>
     <t>при нажатии на кнопки learn more ничего не происходит</t>
   </si>
@@ -664,6 +664,12 @@
   </si>
   <si>
     <t>Vanya Total</t>
+  </si>
+  <si>
+    <t>Прикольно было бы показывать в табе сколько есть комментариев</t>
+  </si>
+  <si>
+    <t>Чтоб по открытию одного фильтра - другие закрывались</t>
   </si>
 </sst>
 </file>
@@ -2400,7 +2406,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:I38" firstHeaderRow="2" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -5915,7 +5921,9 @@
       <c r="C52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="4"/>
+      <c r="D52" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="E52" s="4" t="s">
         <v>80</v>
       </c>
@@ -6522,7 +6530,7 @@
         <v>11</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>97</v>
@@ -7217,7 +7225,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>2</v>
       </c>
@@ -7238,7 +7246,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>2</v>
       </c>
@@ -7259,7 +7267,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>2</v>
       </c>
@@ -7280,7 +7288,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>2</v>
       </c>
@@ -7301,7 +7309,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>2</v>
       </c>
@@ -7322,7 +7330,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>2</v>
       </c>
@@ -7343,7 +7351,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>3</v>
       </c>
@@ -7364,7 +7372,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>2</v>
       </c>
@@ -7387,7 +7395,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>2</v>
       </c>
@@ -7408,7 +7416,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>3</v>
       </c>
@@ -7429,7 +7437,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>2</v>
       </c>
@@ -7450,25 +7458,51 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="6"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="4"/>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="3"/>
+      <c r="E124" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="G124" s="3"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A125" s="6"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="4"/>
+      <c r="H124" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D125" s="4"/>
-      <c r="E125" s="4"/>
-      <c r="F125" s="3"/>
+      <c r="E125" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="G125" s="3"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H125" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
       <c r="B126" s="3"/>
       <c r="C126" s="4"/>
@@ -7477,7 +7511,7 @@
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
       <c r="B127" s="3"/>
       <c r="C127" s="4"/>
@@ -7486,7 +7520,7 @@
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
       <c r="B128" s="3"/>
       <c r="C128" s="4"/>

</xml_diff>

<commit_message>
code refactor - round 1
</commit_message>
<xml_diff>
--- a/Temp/To-Fix.xlsx
+++ b/Temp/To-Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VLAD\IT\DAN_IT\FEM3-FINAL-PROJECT\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364057D6-5151-4806-B6B0-D89116D26631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4E9351-1E04-44DD-931B-10BD65FE8D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F003A8AA-A7D0-4069-AA6E-59105AA6D065}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId3"/>
+    <pivotCache cacheId="19" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="228">
   <si>
     <t>при нажатии на кнопки learn more ничего не происходит</t>
   </si>
@@ -712,6 +712,18 @@
   </si>
   <si>
     <t>рандомизировать товары, товары которые отсутствуют - в конце</t>
+  </si>
+  <si>
+    <t>handleSubmit в defaultProps убивает функцию submit</t>
+  </si>
+  <si>
+    <t>default values в форме не воспринимаются, пока на них не ступишь</t>
+  </si>
+  <si>
+    <t>не подтягивается пол пользователя</t>
+  </si>
+  <si>
+    <t>container for checkout</t>
   </si>
 </sst>
 </file>
@@ -843,7 +855,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2451,7 +2477,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:I38" firstHeaderRow="2" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -2760,47 +2786,75 @@
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <formats count="45">
-    <format dxfId="52">
+    <format dxfId="54">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="53">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="52">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="51">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="50">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="49">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="48">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="45">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="44">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="43">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
@@ -2811,7 +2865,7 @@
             <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -2819,13 +2873,12 @@
     <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
-          <reference field="2" count="3">
+          <reference field="2" count="2">
             <x v="0"/>
             <x v="1"/>
-            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="1"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -2839,7 +2892,7 @@
             <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="2"/>
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -2847,12 +2900,13 @@
     <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
-          <reference field="2" count="2">
+          <reference field="2" count="3">
             <x v="0"/>
             <x v="1"/>
+            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="3"/>
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -2860,13 +2914,11 @@
     <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
-          <reference field="2" count="3">
+          <reference field="2" count="1">
             <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="4"/>
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -2880,7 +2932,7 @@
             <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="5"/>
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
@@ -2892,7 +2944,7 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="6"/>
+            <x v="8"/>
           </reference>
         </references>
       </pivotArea>
@@ -2900,35 +2952,40 @@
     <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
-          <reference field="2" count="3">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
+          <reference field="2" count="0"/>
           <reference field="4" count="1" selected="0">
-            <x v="7"/>
+            <x v="9"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="1">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="8"/>
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="23"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="0"/>
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
           <reference field="4" count="1" selected="0">
-            <x v="9"/>
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="2">
+            <x v="45"/>
+            <x v="59"/>
           </reference>
         </references>
       </pivotArea>
@@ -2940,37 +2997,6 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1">
-            <x v="23"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="2">
-            <x v="45"/>
-            <x v="59"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
             <x v="1"/>
           </reference>
           <reference field="5" count="5">
@@ -2983,7 +3009,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -3005,18 +3031,58 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="2">
+            <x v="4"/>
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="7">
+            <x v="7"/>
+            <x v="28"/>
+            <x v="36"/>
+            <x v="40"/>
+            <x v="49"/>
+            <x v="56"/>
+            <x v="61"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
             <x v="2"/>
           </reference>
-          <reference field="4" count="1" selected="0">
+          <reference field="5" count="5">
             <x v="1"/>
-          </reference>
-          <reference field="5" count="2">
-            <x v="4"/>
-            <x v="18"/>
+            <x v="33"/>
+            <x v="35"/>
+            <x v="38"/>
+            <x v="39"/>
           </reference>
         </references>
       </pivotArea>
@@ -3028,16 +3094,12 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="5" count="7">
-            <x v="7"/>
-            <x v="28"/>
-            <x v="36"/>
-            <x v="40"/>
-            <x v="49"/>
-            <x v="56"/>
-            <x v="61"/>
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="3">
+            <x v="26"/>
+            <x v="27"/>
+            <x v="41"/>
           </reference>
         </references>
       </pivotArea>
@@ -3049,14 +3111,11 @@
             <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="5" count="5">
-            <x v="1"/>
-            <x v="33"/>
-            <x v="35"/>
-            <x v="38"/>
-            <x v="39"/>
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="2">
+            <x v="11"/>
+            <x v="60"/>
           </reference>
         </references>
       </pivotArea>
@@ -3065,15 +3124,16 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="5" count="3">
-            <x v="26"/>
-            <x v="27"/>
-            <x v="41"/>
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="4">
+            <x v="32"/>
+            <x v="34"/>
+            <x v="51"/>
+            <x v="58"/>
           </reference>
         </references>
       </pivotArea>
@@ -3082,14 +3142,16 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="1"/>
+            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="5" count="2">
-            <x v="11"/>
-            <x v="60"/>
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="4">
+            <x v="0"/>
+            <x v="9"/>
+            <x v="44"/>
+            <x v="68"/>
           </reference>
         </references>
       </pivotArea>
@@ -3098,16 +3160,17 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="5" count="4">
-            <x v="32"/>
-            <x v="34"/>
-            <x v="51"/>
-            <x v="58"/>
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="5">
+            <x v="12"/>
+            <x v="13"/>
+            <x v="20"/>
+            <x v="37"/>
+            <x v="57"/>
           </reference>
         </references>
       </pivotArea>
@@ -3116,16 +3179,14 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="2"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="5" count="4">
-            <x v="0"/>
-            <x v="9"/>
-            <x v="44"/>
-            <x v="68"/>
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="2">
+            <x v="3"/>
+            <x v="17"/>
           </reference>
         </references>
       </pivotArea>
@@ -3134,17 +3195,13 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="5"/>
           </reference>
-          <reference field="5" count="5">
-            <x v="12"/>
-            <x v="13"/>
-            <x v="20"/>
-            <x v="37"/>
-            <x v="57"/>
+          <reference field="5" count="1">
+            <x v="47"/>
           </reference>
         </references>
       </pivotArea>
@@ -3153,14 +3210,13 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="5" count="2">
-            <x v="3"/>
-            <x v="17"/>
+            <x v="6"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="29"/>
           </reference>
         </references>
       </pivotArea>
@@ -3169,13 +3225,14 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="2"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="5" count="1">
-            <x v="47"/>
+            <x v="7"/>
+          </reference>
+          <reference field="5" count="2">
+            <x v="65"/>
+            <x v="66"/>
           </reference>
         </references>
       </pivotArea>
@@ -3184,13 +3241,16 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="5" count="1">
-            <x v="29"/>
+            <x v="7"/>
+          </reference>
+          <reference field="5" count="4">
+            <x v="15"/>
+            <x v="22"/>
+            <x v="24"/>
+            <x v="31"/>
           </reference>
         </references>
       </pivotArea>
@@ -3199,14 +3259,14 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="7"/>
           </reference>
           <reference field="5" count="2">
-            <x v="65"/>
-            <x v="66"/>
+            <x v="14"/>
+            <x v="54"/>
           </reference>
         </references>
       </pivotArea>
@@ -3215,16 +3275,13 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="5" count="4">
-            <x v="15"/>
-            <x v="22"/>
-            <x v="24"/>
-            <x v="31"/>
+            <x v="8"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="50"/>
           </reference>
         </references>
       </pivotArea>
@@ -3233,14 +3290,17 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="5" count="5">
             <x v="2"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="5" count="2">
-            <x v="14"/>
-            <x v="54"/>
+            <x v="21"/>
+            <x v="30"/>
+            <x v="42"/>
+            <x v="46"/>
           </reference>
         </references>
       </pivotArea>
@@ -3249,13 +3309,13 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="8"/>
+            <x v="9"/>
           </reference>
           <reference field="5" count="1">
-            <x v="50"/>
+            <x v="48"/>
           </reference>
         </references>
       </pivotArea>
@@ -3264,17 +3324,15 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="9"/>
           </reference>
-          <reference field="5" count="5">
-            <x v="2"/>
-            <x v="21"/>
-            <x v="30"/>
-            <x v="42"/>
-            <x v="46"/>
+          <reference field="5" count="3">
+            <x v="16"/>
+            <x v="25"/>
+            <x v="67"/>
           </reference>
         </references>
       </pivotArea>
@@ -3283,53 +3341,21 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
-            <x v="1"/>
+            <x v="3"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="9"/>
           </reference>
           <reference field="5" count="1">
-            <x v="48"/>
+            <x v="69"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="11">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-          <reference field="5" count="3">
-            <x v="16"/>
-            <x v="25"/>
-            <x v="67"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="10">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-          <reference field="5" count="1">
-            <x v="69"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
@@ -4850,11 +4876,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B89314-F863-48FB-9933-FEF9A79509A7}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7629,7 +7655,9 @@
       <c r="B133" s="3"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
-      <c r="E133" s="4"/>
+      <c r="E133" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="F133" s="15" t="s">
         <v>212</v>
       </c>
@@ -7640,7 +7668,9 @@
       <c r="B134" s="3"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
-      <c r="E134" s="4"/>
+      <c r="E134" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="F134" s="15" t="s">
         <v>213</v>
       </c>
@@ -7695,7 +7725,9 @@
       <c r="B139" s="3"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
+      <c r="E139" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="F139" s="3" t="s">
         <v>219</v>
       </c>
@@ -7706,7 +7738,9 @@
       <c r="B140" s="3"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
+      <c r="E140" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F140" s="15" t="s">
         <v>220</v>
       </c>
@@ -7717,7 +7751,9 @@
       <c r="B141" s="3"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
-      <c r="E141" s="4"/>
+      <c r="E141" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="F141" s="15" t="s">
         <v>222</v>
       </c>
@@ -7728,7 +7764,9 @@
       <c r="B142" s="3"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
+      <c r="E142" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="F142" s="3" t="s">
         <v>221</v>
       </c>
@@ -7778,7 +7816,9 @@
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
-      <c r="F147" s="3"/>
+      <c r="F147" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="G147" s="3"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -7787,7 +7827,9 @@
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
-      <c r="F148" s="3"/>
+      <c r="F148" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="G148" s="3"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -7796,8 +7838,111 @@
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
-      <c r="F149" s="3"/>
+      <c r="F149" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="G149" s="3"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" s="6"/>
+      <c r="B150" s="3"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G150" s="3"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151" s="6"/>
+      <c r="B151" s="3"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152" s="6"/>
+      <c r="B152" s="3"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A153" s="6"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" s="6"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A155" s="6"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A156" s="6"/>
+      <c r="B156" s="3"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="3"/>
+      <c r="G156" s="3"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A157" s="6"/>
+      <c r="B157" s="3"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A158" s="6"/>
+      <c r="B158" s="3"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A159" s="6"/>
+      <c r="B159" s="3"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A160" s="6"/>
+      <c r="B160" s="3"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G126" xr:uid="{A3563D40-676F-4C25-9A83-F9F0579BBF13}">
@@ -7811,6 +7956,14 @@
     <sortCondition ref="B2:B89"/>
   </sortState>
   <conditionalFormatting sqref="C2:C30 C98:C120 C122:C149 C32:C96">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"med"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"high"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C97">
     <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"med"</formula>
     </cfRule>
@@ -7818,7 +7971,7 @@
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
+  <conditionalFormatting sqref="C31">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"med"</formula>
     </cfRule>
@@ -7826,15 +7979,15 @@
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+  <conditionalFormatting sqref="C121">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"med"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C121">
+  <conditionalFormatting sqref="C150:C160">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"med"</formula>
     </cfRule>

</xml_diff>

<commit_message>
search fixing, small refactoring
</commit_message>
<xml_diff>
--- a/Temp/To-Fix.xlsx
+++ b/Temp/To-Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VLAD\IT\DAN_IT\FEM3-FINAL-PROJECT\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4E9351-1E04-44DD-931B-10BD65FE8D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799AF6EC-F5E4-475E-8736-BACB67353F5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F003A8AA-A7D0-4069-AA6E-59105AA6D065}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="229">
   <si>
     <t>при нажатии на кнопки learn more ничего не происходит</t>
   </si>
@@ -724,6 +724,9 @@
   </si>
   <si>
     <t>container for checkout</t>
+  </si>
+  <si>
+    <t>в сортировке переназвать пустое поле на Default или как-то еще</t>
   </si>
 </sst>
 </file>
@@ -2477,7 +2480,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:I38" firstHeaderRow="2" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -4879,8 +4882,8 @@
   <dimension ref="A1:H160"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7868,8 +7871,12 @@
       <c r="B152" s="3"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
-      <c r="E152" s="4"/>
-      <c r="F152" s="3"/>
+      <c r="E152" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="G152" s="3"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
letters finished, eslint fixing
</commit_message>
<xml_diff>
--- a/Temp/To-Fix.xlsx
+++ b/Temp/To-Fix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VLAD\IT\DAN_IT\FEM3-FINAL-PROJECT\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A235C169-ADEE-4735-AF7F-33B4F318CCF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A991BD40-4912-4FC6-913A-B5E982BAB136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F003A8AA-A7D0-4069-AA6E-59105AA6D065}"/>
   </bookViews>
@@ -17,11 +17,11 @@
     <sheet name="General" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">General!$A$1:$G$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">General!$A$1:$G$148</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="252">
   <si>
     <t>при нажатии на кнопки learn more ничего не происходит</t>
   </si>
@@ -672,9 +672,6 @@
     <t>Payment</t>
   </si>
   <si>
-    <t>Subscription</t>
-  </si>
-  <si>
     <t>Подключить подписку</t>
   </si>
   <si>
@@ -790,6 +787,15 @@
   </si>
   <si>
     <t>Подключить Travis (тест на отдельном репозитории)</t>
+  </si>
+  <si>
+    <t>Письмо с подтверждением заказа, регистрации</t>
+  </si>
+  <si>
+    <t>Зачем нам styleLint? Удалить его?</t>
+  </si>
+  <si>
+    <t>Неправильное отображение новых категорий (products requested)</t>
   </si>
 </sst>
 </file>
@@ -921,716 +927,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="282">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
@@ -1856,7 +1153,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Межерицкий Владислав" refreshedDate="43878.67023773148" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="268" xr:uid="{7E8AF15F-9420-4EE8-B76C-CB7DB2EC26A3}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:F977" sheet="General"/>
+    <worksheetSource ref="A1:F976" sheet="General"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Type" numFmtId="0">
@@ -4233,7 +3530,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AFDB375-AFE2-47F1-BF5D-D23CBEA14432}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:I69" firstHeaderRow="2" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -4685,49 +3982,49 @@
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <formats count="45">
-    <format dxfId="281">
+    <format dxfId="54">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="280">
+    <format dxfId="53">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="279">
+    <format dxfId="52">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="278">
+    <format dxfId="51">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="277">
+    <format dxfId="50">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="276">
+    <format dxfId="49">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="275">
+    <format dxfId="48">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="274">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="273">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="272">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="271">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="3">
@@ -4741,7 +4038,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="270">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="3">
@@ -4755,7 +4052,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="269">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="3">
@@ -4769,7 +4066,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="268">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="2">
@@ -4782,7 +4079,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="267">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="3">
@@ -4796,7 +4093,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="266">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="3">
@@ -4810,7 +4107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="265">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1">
@@ -4822,7 +4119,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="264">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="3">
@@ -4836,7 +4133,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="263">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1">
@@ -4848,7 +4145,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="262">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0"/>
@@ -4858,7 +4155,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="261">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4873,7 +4170,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="260">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4889,7 +4186,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="259">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4908,7 +4205,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="258">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4930,7 +4227,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="257">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4946,7 +4243,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="256">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4967,7 +4264,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="255">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -4986,7 +4283,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="254">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5003,7 +4300,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="253">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5019,7 +4316,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="252">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5037,7 +4334,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="251">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5055,7 +4352,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="250">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5074,7 +4371,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="249">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5090,7 +4387,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="248">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5105,7 +4402,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="247">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5120,7 +4417,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="246">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5136,7 +4433,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="245">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5154,7 +4451,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="244">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5170,7 +4467,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="243">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5185,7 +4482,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="242">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5204,7 +4501,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="241">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5219,7 +4516,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="240">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5236,7 +4533,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="239">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="2" count="1" selected="0">
@@ -5251,10 +4548,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="238">
+    <format dxfId="11">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="237">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
@@ -5622,12 +4919,12 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -5684,7 +4981,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -5692,12 +4989,12 @@
         <v>9</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C17" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -5721,37 +5018,37 @@
         <v>11</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C20" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C21" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C22" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C23" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C24" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C25" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -5759,7 +5056,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -5783,7 +5080,7 @@
         <v>11</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -5822,27 +5119,27 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C33" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C34" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C35" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C36" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C37" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -5860,7 +5157,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C40" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -5883,7 +5180,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C44" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -5907,7 +5204,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -5956,7 +5253,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C53" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -6050,22 +5347,22 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C65" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C66" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C67" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
@@ -6596,11 +5893,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B89314-F863-48FB-9933-FEF9A79509A7}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H247"/>
+  <dimension ref="A1:H246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F144" sqref="F144"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6685,7 +5982,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>98</v>
       </c>
@@ -6706,7 +6003,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>98</v>
       </c>
@@ -6727,7 +6024,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>98</v>
       </c>
@@ -6748,7 +6045,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>97</v>
       </c>
@@ -6769,7 +6066,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>97</v>
       </c>
@@ -6790,7 +6087,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>97</v>
       </c>
@@ -6811,7 +6108,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
@@ -7031,7 +6328,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
@@ -7046,7 +6343,7 @@
         <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>192</v>
@@ -7073,7 +6370,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>3</v>
       </c>
@@ -7142,7 +6439,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
@@ -7159,7 +6456,7 @@
         <v>61</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>192</v>
@@ -7364,7 +6661,7 @@
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
@@ -7452,7 +6749,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>2</v>
       </c>
@@ -7519,7 +6816,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>3</v>
       </c>
@@ -8372,7 +7669,7 @@
       </c>
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>2</v>
       </c>
@@ -8389,7 +7686,7 @@
         <v>76</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G81" s="14" t="s">
         <v>192</v>
@@ -8496,12 +7793,14 @@
       <c r="C86" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="E86" s="4" t="s">
         <v>78</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>119</v>
+        <v>249</v>
       </c>
       <c r="G86" s="14" t="s">
         <v>192</v>
@@ -8595,7 +7894,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>2</v>
       </c>
@@ -8610,7 +7909,7 @@
         <v>40</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G91" s="14" t="s">
         <v>192</v>
@@ -8660,7 +7959,7 @@
       </c>
       <c r="G93" s="14"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>3</v>
       </c>
@@ -8675,7 +7974,7 @@
         <v>61</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G94" s="14" t="s">
         <v>192</v>
@@ -8870,7 +8169,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>2</v>
       </c>
@@ -8960,7 +8259,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>3</v>
       </c>
@@ -9006,7 +8305,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>2</v>
       </c>
@@ -9117,7 +8416,7 @@
       </c>
       <c r="G114" s="3"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>2</v>
       </c>
@@ -9138,7 +8437,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>2</v>
       </c>
@@ -9159,7 +8458,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>2</v>
       </c>
@@ -9180,7 +8479,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>3</v>
       </c>
@@ -9251,7 +8550,9 @@
       <c r="C121" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D121" s="4"/>
+      <c r="D121" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="E121" s="4" t="s">
         <v>78</v>
       </c>
@@ -9262,7 +8563,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>3</v>
       </c>
@@ -9304,7 +8605,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>2</v>
       </c>
@@ -9369,12 +8670,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B127" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>9</v>
@@ -9390,12 +8691,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>11</v>
@@ -9405,13 +8706,13 @@
         <v>48</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>2</v>
       </c>
@@ -9426,13 +8727,13 @@
         <v>107</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>2</v>
       </c>
@@ -9447,18 +8748,18 @@
         <v>48</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>11</v>
@@ -9468,18 +8769,18 @@
         <v>48</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>11</v>
@@ -9489,18 +8790,18 @@
         <v>48</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>11</v>
@@ -9510,13 +8811,13 @@
         <v>107</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>2</v>
       </c>
@@ -9531,13 +8832,13 @@
         <v>48</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>2</v>
       </c>
@@ -9552,13 +8853,13 @@
         <v>94</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>3</v>
       </c>
@@ -9573,13 +8874,13 @@
         <v>61</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
         <v>2</v>
       </c>
@@ -9594,13 +8895,13 @@
         <v>107</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
         <v>2</v>
       </c>
@@ -9615,7 +8916,7 @@
         <v>107</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G138" s="3" t="s">
         <v>132</v>
@@ -9638,13 +8939,13 @@
         <v>40</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G139" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
         <v>2</v>
       </c>
@@ -9659,13 +8960,13 @@
         <v>48</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G140" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
         <v>3</v>
       </c>
@@ -9680,13 +8981,13 @@
         <v>107</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>2</v>
       </c>
@@ -9701,13 +9002,13 @@
         <v>107</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G142" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>2</v>
       </c>
@@ -9728,19 +9029,19 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="F144" s="3" t="s">
         <v>211</v>
@@ -9749,7 +9050,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
         <v>2</v>
       </c>
@@ -9761,7 +9062,7 @@
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="F145" s="3" t="s">
         <v>212</v>
@@ -9770,7 +9071,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
         <v>2</v>
       </c>
@@ -9778,11 +9079,11 @@
         <v>221</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>213</v>
@@ -9791,7 +9092,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
         <v>2</v>
       </c>
@@ -9812,7 +9113,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
         <v>2</v>
       </c>
@@ -9824,35 +9125,23 @@
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
-        <v>132</v>
+        <v>40</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>215</v>
+        <v>248</v>
       </c>
       <c r="G148" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A149" s="6"/>
+      <c r="B149" s="3"/>
+      <c r="C149" s="4"/>
       <c r="D149" s="4"/>
-      <c r="E149" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G149" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="E149" s="4"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
@@ -9878,7 +9167,9 @@
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
-      <c r="F152" s="3"/>
+      <c r="F152" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="G152" s="3"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -9887,7 +9178,9 @@
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
-      <c r="F153" s="3"/>
+      <c r="F153" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="G153" s="3"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -10727,71 +10020,60 @@
       <c r="F246" s="3"/>
       <c r="G246" s="3"/>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A247" s="6"/>
-      <c r="B247" s="3"/>
-      <c r="C247" s="4"/>
-      <c r="D247" s="4"/>
-      <c r="E247" s="4"/>
-      <c r="F247" s="3"/>
-      <c r="G247" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G142" xr:uid="{B70710B8-4FF9-40D0-AEFA-E87CE3CC0CF9}">
+  <autoFilter ref="A1:G148" xr:uid="{B70710B8-4FF9-40D0-AEFA-E87CE3CC0CF9}">
     <filterColumn colId="3">
       <filters blank="1">
         <filter val="in progress"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Anya / Vlad"/>
+        <filter val="Vlad"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F85">
     <sortCondition ref="B2:B85"/>
   </sortState>
-  <conditionalFormatting sqref="C91:C109 C2:C89 C111:C141 C143">
-    <cfRule type="cellIs" dxfId="236" priority="19" operator="equal">
+  <conditionalFormatting sqref="C91:C109 C2:C89 C111:C141 C143:C150">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"med"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="234" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"med"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C110">
-    <cfRule type="cellIs" dxfId="232" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"med"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C144:C151">
-    <cfRule type="cellIs" dxfId="230" priority="5" operator="equal">
+  <conditionalFormatting sqref="C151:C246">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"med"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="6" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C152:C247">
-    <cfRule type="cellIs" dxfId="228" priority="3" operator="equal">
-      <formula>"med"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C142">
-    <cfRule type="cellIs" dxfId="226" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"med"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"high"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>